<commit_message>
Update default trade elasticities
Reduce Armington elasticities between domestic and imported products
from 5 to 3. For a range of utility products (electricity and etc) make
trade relatively inelastic. The new values are based on assumptions used
by EPPA model.
</commit_message>
<xml_diff>
--- a/project_example/00_base_model_setup/data/Eldata.xlsx
+++ b/project_example/00_base_model_setup/data/Eldata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="20115" windowHeight="9780" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="20115" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="elasFU_CES" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="96">
   <si>
     <t>elasIU_DM</t>
   </si>
@@ -296,6 +296,18 @@
   </si>
   <si>
     <t>"Worldscan: a model for international economic policy analysis"</t>
+  </si>
+  <si>
+    <t>The values are taken and assigned to the model product from EPPA model description (p. 17)</t>
+  </si>
+  <si>
+    <t>Sergey Paltsev, John M. Reilly, Henry D. Jacoby, Richard S. Eckaus, James McFarland, Marcus Sarofim, Malcolm Asadoorian and Mustafa Babiker, 2005</t>
+  </si>
+  <si>
+    <t>The MIT Emissions Prediction and Policy Analysis (EPPA) Model: Version 4</t>
+  </si>
+  <si>
+    <t>Report No. 125</t>
   </si>
 </sst>
 </file>
@@ -342,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -351,6 +363,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -654,7 +667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -705,7 +718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1126,15 +1139,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A36"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1147,16 +1158,19 @@
       <c r="E1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H1" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B2">
-        <v>5</v>
-      </c>
-      <c r="C2">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="C2" s="4">
+        <v>3</v>
       </c>
       <c r="D2">
         <v>5</v>
@@ -1164,16 +1178,17 @@
       <c r="E2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>5</v>
+      <c r="B3" s="4">
+        <v>3</v>
+      </c>
+      <c r="C3" s="4">
+        <v>3</v>
       </c>
       <c r="D3">
         <v>5</v>
@@ -1181,16 +1196,19 @@
       <c r="E3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H3" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4">
-        <v>5</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
+      <c r="B4" s="4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4">
+        <v>3</v>
       </c>
       <c r="D4">
         <v>5</v>
@@ -1198,16 +1216,19 @@
       <c r="E4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H4" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
+      <c r="B5" s="4">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4">
+        <v>3</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -1215,16 +1236,19 @@
       <c r="E5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H5" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
+      <c r="B6" s="4">
+        <v>3</v>
+      </c>
+      <c r="C6" s="4">
+        <v>3</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -1233,15 +1257,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B7">
-        <v>5</v>
-      </c>
-      <c r="C7">
-        <v>5</v>
+      <c r="B7" s="4">
+        <v>3</v>
+      </c>
+      <c r="C7" s="4">
+        <v>3</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -1250,15 +1274,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B8">
-        <v>5</v>
-      </c>
-      <c r="C8">
-        <v>5</v>
+      <c r="B8" s="4">
+        <v>3</v>
+      </c>
+      <c r="C8" s="4">
+        <v>3</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -1267,15 +1291,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B9">
-        <v>5</v>
-      </c>
-      <c r="C9">
-        <v>5</v>
+      <c r="B9" s="4">
+        <v>3</v>
+      </c>
+      <c r="C9" s="4">
+        <v>3</v>
       </c>
       <c r="D9">
         <v>5</v>
@@ -1284,15 +1308,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B10">
-        <v>5</v>
-      </c>
-      <c r="C10">
-        <v>5</v>
+      <c r="B10" s="4">
+        <v>3</v>
+      </c>
+      <c r="C10" s="4">
+        <v>3</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -1301,15 +1325,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B11">
-        <v>5</v>
-      </c>
-      <c r="C11">
-        <v>5</v>
+      <c r="B11" s="4">
+        <v>3</v>
+      </c>
+      <c r="C11" s="4">
+        <v>3</v>
       </c>
       <c r="D11">
         <v>5</v>
@@ -1318,15 +1342,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B12">
-        <v>5</v>
-      </c>
-      <c r="C12">
-        <v>5</v>
+      <c r="B12" s="4">
+        <v>3</v>
+      </c>
+      <c r="C12" s="4">
+        <v>3</v>
       </c>
       <c r="D12">
         <v>5</v>
@@ -1335,15 +1359,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B13">
-        <v>5</v>
-      </c>
-      <c r="C13">
-        <v>5</v>
+      <c r="B13" s="4">
+        <v>3</v>
+      </c>
+      <c r="C13" s="4">
+        <v>3</v>
       </c>
       <c r="D13">
         <v>5</v>
@@ -1352,15 +1376,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B14">
-        <v>5</v>
-      </c>
-      <c r="C14">
-        <v>5</v>
+      <c r="B14" s="4">
+        <v>3</v>
+      </c>
+      <c r="C14" s="4">
+        <v>3</v>
       </c>
       <c r="D14">
         <v>5</v>
@@ -1369,15 +1393,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B15">
-        <v>5</v>
-      </c>
-      <c r="C15">
-        <v>5</v>
+      <c r="B15" s="4">
+        <v>3</v>
+      </c>
+      <c r="C15" s="4">
+        <v>3</v>
       </c>
       <c r="D15">
         <v>5</v>
@@ -1386,15 +1410,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B16">
-        <v>5</v>
-      </c>
-      <c r="C16">
-        <v>5</v>
+      <c r="B16" s="4">
+        <v>3</v>
+      </c>
+      <c r="C16" s="4">
+        <v>3</v>
       </c>
       <c r="D16">
         <v>5</v>
@@ -1407,11 +1431,11 @@
       <c r="A17" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B17">
-        <v>5</v>
-      </c>
-      <c r="C17">
-        <v>5</v>
+      <c r="B17" s="4">
+        <v>3</v>
+      </c>
+      <c r="C17" s="4">
+        <v>3</v>
       </c>
       <c r="D17">
         <v>5</v>
@@ -1424,11 +1448,11 @@
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B18">
-        <v>5</v>
-      </c>
-      <c r="C18">
-        <v>5</v>
+      <c r="B18" s="4">
+        <v>3</v>
+      </c>
+      <c r="C18" s="4">
+        <v>3</v>
       </c>
       <c r="D18">
         <v>5</v>
@@ -1441,11 +1465,11 @@
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B19">
-        <v>5</v>
-      </c>
-      <c r="C19">
-        <v>5</v>
+      <c r="B19" s="4">
+        <v>3</v>
+      </c>
+      <c r="C19" s="4">
+        <v>3</v>
       </c>
       <c r="D19">
         <v>5</v>
@@ -1458,11 +1482,11 @@
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B20">
-        <v>5</v>
-      </c>
-      <c r="C20">
-        <v>5</v>
+      <c r="B20" s="4">
+        <v>3</v>
+      </c>
+      <c r="C20" s="4">
+        <v>3</v>
       </c>
       <c r="D20">
         <v>5</v>
@@ -1475,11 +1499,11 @@
       <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B21">
-        <v>5</v>
-      </c>
-      <c r="C21">
-        <v>5</v>
+      <c r="B21" s="4">
+        <v>3</v>
+      </c>
+      <c r="C21" s="4">
+        <v>3</v>
       </c>
       <c r="D21">
         <v>5</v>
@@ -1492,11 +1516,11 @@
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B22">
-        <v>5</v>
-      </c>
-      <c r="C22">
-        <v>5</v>
+      <c r="B22" s="4">
+        <v>3</v>
+      </c>
+      <c r="C22" s="4">
+        <v>3</v>
       </c>
       <c r="D22">
         <v>5</v>
@@ -1509,11 +1533,11 @@
       <c r="A23" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B23">
-        <v>5</v>
-      </c>
-      <c r="C23">
-        <v>5</v>
+      <c r="B23" s="4">
+        <v>3</v>
+      </c>
+      <c r="C23" s="4">
+        <v>3</v>
       </c>
       <c r="D23">
         <v>5</v>
@@ -1526,11 +1550,11 @@
       <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B24">
-        <v>5</v>
-      </c>
-      <c r="C24">
-        <v>5</v>
+      <c r="B24" s="4">
+        <v>3</v>
+      </c>
+      <c r="C24" s="4">
+        <v>3</v>
       </c>
       <c r="D24">
         <v>5</v>
@@ -1543,96 +1567,96 @@
       <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B25">
-        <v>5</v>
-      </c>
-      <c r="C25">
-        <v>5</v>
+      <c r="B25" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0.3</v>
       </c>
       <c r="D25">
-        <v>5</v>
-      </c>
-      <c r="E25">
-        <v>5</v>
+        <v>0.5</v>
+      </c>
+      <c r="E25" s="4">
+        <v>0.5</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B26">
-        <v>5</v>
-      </c>
-      <c r="C26">
-        <v>5</v>
-      </c>
-      <c r="D26">
-        <v>5</v>
-      </c>
-      <c r="E26">
-        <v>5</v>
+      <c r="B26" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="C26" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="D26" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E26" s="4">
+        <v>0.5</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B27">
-        <v>5</v>
-      </c>
-      <c r="C27">
-        <v>5</v>
-      </c>
-      <c r="D27">
-        <v>5</v>
-      </c>
-      <c r="E27">
-        <v>5</v>
+      <c r="B27" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E27" s="4">
+        <v>0.5</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B28">
-        <v>5</v>
-      </c>
-      <c r="C28">
-        <v>5</v>
-      </c>
-      <c r="D28">
-        <v>5</v>
-      </c>
-      <c r="E28">
-        <v>5</v>
+      <c r="B28" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="C28" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="D28" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E28" s="4">
+        <v>0.5</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B29">
-        <v>5</v>
-      </c>
-      <c r="C29">
-        <v>5</v>
-      </c>
-      <c r="D29">
-        <v>5</v>
-      </c>
-      <c r="E29">
-        <v>5</v>
+      <c r="B29" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="C29" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="D29" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E29" s="4">
+        <v>0.5</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B30">
-        <v>5</v>
-      </c>
-      <c r="C30">
-        <v>5</v>
+      <c r="B30" s="4">
+        <v>3</v>
+      </c>
+      <c r="C30" s="4">
+        <v>3</v>
       </c>
       <c r="D30">
         <v>5</v>
@@ -1645,11 +1669,11 @@
       <c r="A31" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B31">
-        <v>5</v>
-      </c>
-      <c r="C31">
-        <v>5</v>
+      <c r="B31" s="4">
+        <v>3</v>
+      </c>
+      <c r="C31" s="4">
+        <v>3</v>
       </c>
       <c r="D31">
         <v>5</v>
@@ -1662,11 +1686,11 @@
       <c r="A32" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B32">
-        <v>5</v>
-      </c>
-      <c r="C32">
-        <v>5</v>
+      <c r="B32" s="4">
+        <v>3</v>
+      </c>
+      <c r="C32" s="4">
+        <v>3</v>
       </c>
       <c r="D32">
         <v>5</v>
@@ -1679,11 +1703,11 @@
       <c r="A33" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B33">
-        <v>5</v>
-      </c>
-      <c r="C33">
-        <v>5</v>
+      <c r="B33" s="4">
+        <v>3</v>
+      </c>
+      <c r="C33" s="4">
+        <v>3</v>
       </c>
       <c r="D33">
         <v>5</v>
@@ -1696,11 +1720,11 @@
       <c r="A34" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B34">
-        <v>5</v>
-      </c>
-      <c r="C34">
-        <v>5</v>
+      <c r="B34" s="4">
+        <v>3</v>
+      </c>
+      <c r="C34" s="4">
+        <v>3</v>
       </c>
       <c r="D34">
         <v>5</v>
@@ -1713,11 +1737,11 @@
       <c r="A35" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B35">
-        <v>5</v>
-      </c>
-      <c r="C35">
-        <v>5</v>
+      <c r="B35" s="4">
+        <v>3</v>
+      </c>
+      <c r="C35" s="4">
+        <v>3</v>
       </c>
       <c r="D35">
         <v>5</v>
@@ -1730,11 +1754,11 @@
       <c r="A36" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B36">
-        <v>5</v>
-      </c>
-      <c r="C36">
-        <v>5</v>
+      <c r="B36" s="4">
+        <v>3</v>
+      </c>
+      <c r="C36" s="4">
+        <v>3</v>
       </c>
       <c r="D36">
         <v>5</v>

</xml_diff>

<commit_message>
Change database to aggregated database for opensource version of model
</commit_message>
<xml_diff>
--- a/project_example/00_base_model_setup/data/Eldata.xlsx
+++ b/project_example/00_base_model_setup/data/Eldata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boonmanhj\Documents\Gitlab\tno-eco-mod-ci\project_example\00_base_model_setup\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{827D7B25-CEF5-4A76-A207-1FE0978E9773}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A78F3D-8BCE-4FE5-93C5-7974D83BDBBC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="elasFU_CES" sheetId="5" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="55">
   <si>
     <t>elasIU_DM</t>
   </si>
@@ -174,30 +174,6 @@
     <t>pHTWT</t>
   </si>
   <si>
-    <t>pOIL</t>
-  </si>
-  <si>
-    <t>pGSL</t>
-  </si>
-  <si>
-    <t>pDSL</t>
-  </si>
-  <si>
-    <t>pHDI</t>
-  </si>
-  <si>
-    <t>pNG</t>
-  </si>
-  <si>
-    <t>pCOA</t>
-  </si>
-  <si>
-    <t>pBIO</t>
-  </si>
-  <si>
-    <t>pFUL</t>
-  </si>
-  <si>
     <t>iAGRI</t>
   </si>
   <si>
@@ -220,6 +196,9 @@
   </si>
   <si>
     <t>iH2</t>
+  </si>
+  <si>
+    <t>pENER</t>
   </si>
 </sst>
 </file>
@@ -670,7 +649,7 @@
   <dimension ref="A1:V46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A17"/>
+      <selection activeCell="A11" sqref="A11:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -810,7 +789,7 @@
     </row>
     <row r="10" spans="1:22">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B10">
         <v>0.97</v>
@@ -823,99 +802,51 @@
       <c r="V10" s="4"/>
     </row>
     <row r="11" spans="1:22">
-      <c r="A11" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="4">
-        <v>0.97</v>
-      </c>
-      <c r="C11">
-        <v>-1.54</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="B11" s="4"/>
       <c r="T11" s="1"/>
       <c r="U11" s="4"/>
       <c r="V11" s="4"/>
     </row>
     <row r="12" spans="1:22">
-      <c r="A12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="4">
-        <v>0.97</v>
-      </c>
-      <c r="C12">
-        <v>-1.54</v>
-      </c>
+      <c r="A12" s="1"/>
+      <c r="B12" s="4"/>
       <c r="T12" s="1"/>
       <c r="U12" s="4"/>
       <c r="V12" s="4"/>
     </row>
     <row r="13" spans="1:22">
-      <c r="A13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" s="4">
-        <v>0.97</v>
-      </c>
-      <c r="C13">
-        <v>-1.54</v>
-      </c>
+      <c r="A13" s="1"/>
+      <c r="B13" s="4"/>
       <c r="T13" s="1"/>
       <c r="U13" s="4"/>
       <c r="V13" s="4"/>
     </row>
     <row r="14" spans="1:22">
-      <c r="A14" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="4">
-        <v>0.97</v>
-      </c>
-      <c r="C14" s="4">
-        <v>-1.54</v>
-      </c>
+      <c r="A14" s="1"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
       <c r="T14" s="1"/>
       <c r="U14" s="4"/>
       <c r="V14" s="4"/>
     </row>
     <row r="15" spans="1:22">
-      <c r="A15" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="4">
-        <v>0.97</v>
-      </c>
-      <c r="C15">
-        <v>-1.54</v>
-      </c>
+      <c r="A15" s="1"/>
+      <c r="B15" s="4"/>
       <c r="T15" s="1"/>
       <c r="U15" s="4"/>
       <c r="V15" s="4"/>
     </row>
     <row r="16" spans="1:22">
-      <c r="A16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" s="4">
-        <v>0.97</v>
-      </c>
-      <c r="C16">
-        <v>-1.54</v>
-      </c>
+      <c r="A16" s="1"/>
+      <c r="B16" s="4"/>
       <c r="T16" s="1"/>
       <c r="U16" s="4"/>
       <c r="V16" s="4"/>
     </row>
     <row r="17" spans="1:22">
-      <c r="A17" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="4">
-        <v>0.97</v>
-      </c>
-      <c r="C17">
-        <v>-1.54</v>
-      </c>
+      <c r="A17" s="1"/>
+      <c r="B17" s="4"/>
       <c r="T17" s="1"/>
       <c r="U17" s="4"/>
       <c r="V17" s="4"/>
@@ -1001,8 +932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1172,7 +1103,7 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B10" s="4">
         <v>3</v>
@@ -1188,21 +1119,11 @@
       </c>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="4">
-        <v>3</v>
-      </c>
-      <c r="C11" s="4">
-        <v>3</v>
-      </c>
-      <c r="D11" s="4">
-        <v>5</v>
-      </c>
-      <c r="E11" s="4">
-        <v>5</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
       <c r="I11" s="1"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
@@ -1210,21 +1131,11 @@
       <c r="M11" s="4"/>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="4">
-        <v>3</v>
-      </c>
-      <c r="C12" s="4">
-        <v>3</v>
-      </c>
-      <c r="D12" s="4">
-        <v>5</v>
-      </c>
-      <c r="E12" s="4">
-        <v>5</v>
-      </c>
+      <c r="A12" s="1"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
       <c r="I12" s="1"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
@@ -1232,21 +1143,11 @@
       <c r="M12" s="4"/>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" s="4">
-        <v>3</v>
-      </c>
-      <c r="C13" s="4">
-        <v>3</v>
-      </c>
-      <c r="D13" s="4">
-        <v>5</v>
-      </c>
-      <c r="E13" s="4">
-        <v>5</v>
-      </c>
+      <c r="A13" s="1"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
       <c r="I13" s="1"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
@@ -1254,21 +1155,11 @@
       <c r="M13" s="4"/>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="4">
-        <v>3</v>
-      </c>
-      <c r="C14" s="4">
-        <v>3</v>
-      </c>
-      <c r="D14" s="4">
-        <v>5</v>
-      </c>
-      <c r="E14" s="4">
-        <v>5</v>
-      </c>
+      <c r="A14" s="1"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
       <c r="I14" s="1"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
@@ -1276,21 +1167,11 @@
       <c r="M14" s="4"/>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="4">
-        <v>3</v>
-      </c>
-      <c r="C15" s="4">
-        <v>3</v>
-      </c>
-      <c r="D15" s="4">
-        <v>5</v>
-      </c>
-      <c r="E15" s="4">
-        <v>5</v>
-      </c>
+      <c r="A15" s="1"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
       <c r="I15" s="1"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
@@ -1298,21 +1179,11 @@
       <c r="M15" s="4"/>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" s="4">
-        <v>3</v>
-      </c>
-      <c r="C16" s="4">
-        <v>3</v>
-      </c>
-      <c r="D16" s="4">
-        <v>5</v>
-      </c>
-      <c r="E16" s="4">
-        <v>5</v>
-      </c>
+      <c r="A16" s="1"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
       <c r="I16" s="1"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
@@ -1320,21 +1191,11 @@
       <c r="M16" s="4"/>
     </row>
     <row r="17" spans="1:13">
-      <c r="A17" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="4">
-        <v>3</v>
-      </c>
-      <c r="C17" s="4">
-        <v>3</v>
-      </c>
-      <c r="D17" s="4">
-        <v>5</v>
-      </c>
-      <c r="E17" s="4">
-        <v>5</v>
-      </c>
+      <c r="A17" s="1"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
       <c r="I17" s="1"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
@@ -1495,7 +1356,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B2" s="4">
         <v>0.29535</v>
@@ -1503,7 +1364,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B3" s="4">
         <v>1.2801</v>
@@ -1511,7 +1372,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B4" s="4">
         <v>0.31059999999999999</v>
@@ -1519,7 +1380,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B5" s="4">
         <v>0.5952599999999999</v>
@@ -1527,7 +1388,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B6" s="4">
         <v>0.28660000000000002</v>
@@ -1543,7 +1404,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B8" s="4">
         <v>0.30209999999999998</v>
@@ -1559,7 +1420,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B10" s="4">
         <v>0.57545000000000002</v>
@@ -1647,7 +1508,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B21" s="4">
         <v>0.30209999999999998</v>
@@ -1733,7 +1594,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -1744,7 +1605,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B3" s="4">
         <v>1</v>
@@ -1755,7 +1616,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B4" s="4">
         <v>1</v>
@@ -1766,7 +1627,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B5" s="4">
         <v>1</v>
@@ -1777,7 +1638,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B6" s="4">
         <v>1</v>
@@ -1799,7 +1660,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B8" s="4">
         <v>1</v>
@@ -1821,7 +1682,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B10" s="4">
         <v>1</v>
@@ -1942,7 +1803,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B21" s="4">
         <v>1</v>
@@ -2043,7 +1904,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:W46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -2076,7 +1937,7 @@
     </row>
     <row r="2" spans="1:23">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B2" s="4">
         <v>2.84815</v>
@@ -2104,7 +1965,7 @@
     </row>
     <row r="3" spans="1:23">
       <c r="A3" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B3" s="4">
         <v>0.53959999999999997</v>
@@ -2132,7 +1993,7 @@
     </row>
     <row r="4" spans="1:23">
       <c r="A4" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B4" s="4">
         <v>7.8575999999999997</v>
@@ -2160,7 +2021,7 @@
     </row>
     <row r="5" spans="1:23">
       <c r="A5" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B5" s="4">
         <v>0.24174999999999999</v>
@@ -2188,7 +2049,7 @@
     </row>
     <row r="6" spans="1:23">
       <c r="A6" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B6" s="4">
         <v>0.86909999999999998</v>
@@ -2244,7 +2105,7 @@
     </row>
     <row r="8" spans="1:23">
       <c r="A8" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B8" s="4">
         <v>0.2757</v>
@@ -2300,7 +2161,7 @@
     </row>
     <row r="10" spans="1:23">
       <c r="A10" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B10" s="4">
         <v>0.72006666666666652</v>
@@ -2608,7 +2469,7 @@
     </row>
     <row r="21" spans="1:23">
       <c r="A21" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B21" s="4">
         <v>0.2757</v>
@@ -2832,7 +2693,7 @@
     </row>
     <row r="2" spans="1:21">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -2856,7 +2717,7 @@
     </row>
     <row r="3" spans="1:21">
       <c r="A3" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B3" s="4">
         <v>1</v>
@@ -2881,7 +2742,7 @@
     </row>
     <row r="4" spans="1:21">
       <c r="A4" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B4" s="4">
         <v>1</v>
@@ -2906,7 +2767,7 @@
     </row>
     <row r="5" spans="1:21">
       <c r="A5" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B5" s="4">
         <v>1</v>
@@ -2931,7 +2792,7 @@
     </row>
     <row r="6" spans="1:21">
       <c r="A6" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B6" s="4">
         <v>1</v>
@@ -2981,7 +2842,7 @@
     </row>
     <row r="8" spans="1:21">
       <c r="A8" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B8" s="4">
         <v>1</v>
@@ -3031,7 +2892,7 @@
     </row>
     <row r="10" spans="1:21">
       <c r="A10" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B10" s="4">
         <v>1</v>
@@ -3274,7 +3135,7 @@
     </row>
     <row r="21" spans="1:16">
       <c r="A21" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B21" s="4">
         <v>1</v>

</xml_diff>